<commit_message>
update list of stocks
</commit_message>
<xml_diff>
--- a/chair/EWG 25 09 Stock allocation list.xlsx
+++ b/chair/EWG 25 09 Stock allocation list.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,30 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
-  <si>
-    <t>MEETING:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STECF EWG 25 09  Stock assessments in the West Mediterranean Sea 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JRC Ispra 06/09/2025 - 12/09/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STOCK ASSESSMENT DURING EWG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STOCK for ad hoc contract (max 14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t>Email</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock coord</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 model</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
   <si>
     <t xml:space="preserve">NEP 9 </t>
@@ -123,9 +117,6 @@
     <t xml:space="preserve">NEP 5</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>FARRE</t>
   </si>
   <si>
@@ -312,23 +303,41 @@
     <t>PIERUCCI</t>
   </si>
   <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea.PIERUCCI@ec.europa.eu </t>
+  </si>
+  <si>
     <t xml:space="preserve">DPS 5-6-7</t>
   </si>
   <si>
+    <t xml:space="preserve">MANTOPOULOU PALOUKA</t>
+  </si>
+  <si>
     <t>DANAI</t>
   </si>
   <si>
+    <t xml:space="preserve">Danai.MANTOPOULOU-PALOUKA@ec.europa.eu </t>
+  </si>
+  <si>
     <t xml:space="preserve">MUT 10</t>
   </si>
   <si>
+    <t xml:space="preserve">RINCON HIDALGO</t>
+  </si>
+  <si>
     <t>MARGHERITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margarita.RINCON-HIDALGO@ec.europa.eu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -340,51 +349,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.000000"/>
-      <color indexed="65"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11.000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="0"/>
-        <bgColor theme="0" tint="0"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -400,27 +371,10 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -933,520 +887,518 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1">
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="30.65234375"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="31.22265625"/>
-    <col customWidth="1" min="3" max="3" width="30.08984375"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" width="11.54296875"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" width="38.81640625"/>
+    <col customWidth="1" min="2" max="2" width="20.7109375"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="21.97265625"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="23.36328125"/>
+    <col customWidth="1" min="5" max="5" width="20.7109375"/>
+    <col customWidth="1" min="6" max="6" width="42.57421875"/>
+    <col customWidth="1" min="7" max="7" width="20.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="C1" s="1" t="s">
+    <row r="1" ht="14.25"/>
+    <row r="2" ht="14.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="20.149999999999999" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="1">
-      <c r="A5" s="6" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+    </row>
+    <row r="4" ht="14.25">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" s="6" customFormat="1">
-      <c r="A6" s="6" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="6" t="s">
+    </row>
+    <row r="5" ht="14.25">
+      <c r="B5"/>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" s="6" customFormat="1">
-      <c r="B7" s="6" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" s="6" customFormat="1">
-      <c r="C8" s="6" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="G6"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" s="6" customFormat="1">
-      <c r="A9" s="6" t="s">
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" s="6" customFormat="1">
-      <c r="A10" s="6" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="C9"/>
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" s="6" customFormat="1">
-      <c r="A11" s="6" t="s">
+      <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="6" t="s">
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" s="6" customFormat="1">
-      <c r="C12" s="6" t="s">
+      <c r="G10"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" s="6" customFormat="1">
-      <c r="A13" s="6" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" s="6" customFormat="1">
-      <c r="A14" s="6" t="s">
+      <c r="F12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="C13"/>
+      <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" s="6" customFormat="1">
-      <c r="A15" s="6" t="s">
+      <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" s="6" customFormat="1">
-      <c r="A16" s="6" t="s">
+      <c r="F14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" s="6" customFormat="1">
-      <c r="C17" s="6" t="s">
+      <c r="G15"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" s="6" customFormat="1">
-      <c r="A18" s="6" t="s">
+      <c r="F16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" s="6" customFormat="1">
-      <c r="A19" s="6" t="s">
+      <c r="E17" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="F17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" s="6" customFormat="1">
-      <c r="A20" s="6" t="s">
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" s="6" customFormat="1">
-      <c r="A21" s="6" t="s">
+      <c r="F19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" s="6" customFormat="1">
-      <c r="A22" s="6" t="s">
+      <c r="E20" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="F20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" s="6" customFormat="1">
-      <c r="A23" s="6" t="s">
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="F21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="G21" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="6" t="s">
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="E22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" s="6" customFormat="1">
-      <c r="A24" s="6" t="s">
+      <c r="F22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E23" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" s="6" customFormat="1">
-      <c r="A25" s="8" t="s">
+      <c r="F23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9" t="s">
+      <c r="G24"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="10" t="s">
+      <c r="C25"/>
+      <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="E25" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" ht="15">
-      <c r="A28" s="10" t="s">
+      <c r="F25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="C26"/>
+      <c r="D26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:D2"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E23"/>
+    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink r:id="rId2" ref="F4"/>
+    <hyperlink r:id="rId3" ref="F5"/>
+    <hyperlink r:id="rId4" ref="F6"/>
+    <hyperlink r:id="rId5" ref="F7"/>
+    <hyperlink r:id="rId6" ref="F8"/>
+    <hyperlink r:id="rId7" ref="F9"/>
+    <hyperlink r:id="rId8" ref="F10"/>
+    <hyperlink r:id="rId9" ref="F11"/>
+    <hyperlink r:id="rId10" ref="F12"/>
+    <hyperlink r:id="rId11" ref="F13"/>
+    <hyperlink r:id="rId12" ref="F14"/>
+    <hyperlink r:id="rId13" ref="F15"/>
+    <hyperlink r:id="rId14" ref="F16"/>
+    <hyperlink r:id="rId15" ref="F17"/>
+    <hyperlink r:id="rId16" ref="F18"/>
+    <hyperlink r:id="rId17" ref="F19"/>
+    <hyperlink r:id="rId18" ref="F20"/>
+    <hyperlink r:id="rId19" ref="F21"/>
+    <hyperlink r:id="rId20" ref="F22"/>
+    <hyperlink r:id="rId21" ref="F23"/>
+    <hyperlink r:id="rId22" ref="F24"/>
+    <hyperlink r:id="rId23" ref="F25"/>
+    <hyperlink r:id="rId24" ref="F26"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated stock assessment summary
</commit_message>
<xml_diff>
--- a/chair/EWG 25 09 Stock allocation list.xlsx
+++ b/chair/EWG 25 09 Stock allocation list.xlsx
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Stock</t>
   </si>
   <si>
+    <t>GSA</t>
+  </si>
+  <si>
     <t>Contract</t>
   </si>
   <si>
@@ -36,6 +39,99 @@
     <t>Data</t>
   </si>
   <si>
+    <t xml:space="preserve">DPS 1</t>
+  </si>
+  <si>
+    <t>MURENU</t>
+  </si>
+  <si>
+    <t>Matteo</t>
+  </si>
+  <si>
+    <t>mmurenu@unica.it</t>
+  </si>
+  <si>
+    <t>a4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEP 5</t>
+  </si>
+  <si>
+    <t>FARRE</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>marc.farre@ieo.csic.es</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUR 5</t>
+  </si>
+  <si>
+    <t>KONRAD</t>
+  </si>
+  <si>
+    <t>Christoph</t>
+  </si>
+  <si>
+    <t>chriskon.official@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARA 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZARAGOZA VILANOVA</t>
+  </si>
+  <si>
+    <t>NúRia</t>
+  </si>
+  <si>
+    <t>nuria.zaragoza@ieo.csic.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUT 6</t>
+  </si>
+  <si>
+    <t>GARCÍA</t>
+  </si>
+  <si>
+    <t>Encarni</t>
+  </si>
+  <si>
+    <t>encarnacion.garcia@ieo.csic.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEP 6</t>
+  </si>
+  <si>
+    <t>TIFOURA</t>
+  </si>
+  <si>
+    <t>Amina</t>
+  </si>
+  <si>
+    <t>amina.tifoura@ieo.csic.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUT 7</t>
+  </si>
+  <si>
+    <t>CERTAIN</t>
+  </si>
+  <si>
+    <t>Gregoire</t>
+  </si>
+  <si>
+    <t>gregoire.certain@ifremer.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEP 9 </t>
   </si>
   <si>
@@ -54,19 +150,160 @@
     <t xml:space="preserve">cat 5</t>
   </si>
   <si>
-    <t xml:space="preserve">MUT 7</t>
-  </si>
-  <si>
-    <t>CERTAIN</t>
-  </si>
-  <si>
-    <t>Gregoire</t>
-  </si>
-  <si>
-    <t>gregoire.certain@ifremer.fr</t>
-  </si>
-  <si>
-    <t>a4a</t>
+    <t xml:space="preserve">MUT 9</t>
+  </si>
+  <si>
+    <t>LIGAS</t>
+  </si>
+  <si>
+    <t>Alessandro</t>
+  </si>
+  <si>
+    <t>ligas@cibm.it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUT 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RINCON HIDALGO</t>
+  </si>
+  <si>
+    <t>MARGHERITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margarita.RINCON-HIDALGO@ec.europa.eu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEP 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEP 11 &amp; MUR 5</t>
+  </si>
+  <si>
+    <t>SCANU</t>
+  </si>
+  <si>
+    <t>Martina</t>
+  </si>
+  <si>
+    <t>martina.scanu@irbim.cnr.it</t>
+  </si>
+  <si>
+    <t>spict</t>
+  </si>
+  <si>
+    <t>ARA1-2</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARRIGA PANISELLO</t>
+  </si>
+  <si>
+    <t>Mariona</t>
+  </si>
+  <si>
+    <t>mariona.garripa@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKE 1-5-6-7  and HKE ad hoc?</t>
+  </si>
+  <si>
+    <t>1-5-6-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKE 1-5-6-7</t>
+  </si>
+  <si>
+    <t>PEREZ-RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>Alfonso</t>
+  </si>
+  <si>
+    <t>alfonso.perez@ieo.csic.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS 5-6-7</t>
+  </si>
+  <si>
+    <t>5-6-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANTOPOULOU PALOUKA</t>
+  </si>
+  <si>
+    <t>DANAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danai.MANTOPOULOU-PALOUKA@ec.europa.eu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARA 6-7</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>COUVE</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>pablo.couve@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPS 8-9-10-11</t>
+  </si>
+  <si>
+    <t>8-9-10-11</t>
+  </si>
+  <si>
+    <t>COSTANTINI</t>
+  </si>
+  <si>
+    <t>Ilaria</t>
+  </si>
+  <si>
+    <t>ilaria.costantini@cnr.it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKE 8-9-10-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKE 8-9-10-11 &amp; MUT 10</t>
+  </si>
+  <si>
+    <t>MUSUMECI</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>clamusu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARA 8-9-10-11</t>
+  </si>
+  <si>
+    <t>ORIO</t>
+  </si>
+  <si>
+    <t>alessandro.orio@slu.se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARS 8-9-10-11</t>
+  </si>
+  <si>
+    <t>PALERMINO</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>antonio.palermino@irbim.cnr.it</t>
   </si>
   <si>
     <t xml:space="preserve">MUT 1</t>
@@ -90,45 +327,6 @@
     <t>cyrine.chenaoui@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">DPS 8-9-10-11</t>
-  </si>
-  <si>
-    <t>COSTANTINI</t>
-  </si>
-  <si>
-    <t>Ilaria</t>
-  </si>
-  <si>
-    <t>ilaria.costantini@cnr.it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARA 6-7</t>
-  </si>
-  <si>
-    <t>COUVE</t>
-  </si>
-  <si>
-    <t>Pablo</t>
-  </si>
-  <si>
-    <t>pablo.couve@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEP 5</t>
-  </si>
-  <si>
-    <t>FARRE</t>
-  </si>
-  <si>
-    <t>Marc</t>
-  </si>
-  <si>
-    <t>marc.farre@ieo.csic.es</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
     <t xml:space="preserve">GAMITO JARDIM</t>
   </si>
   <si>
@@ -138,54 +336,6 @@
     <t>ernesto.jardim@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">MUT 6</t>
-  </si>
-  <si>
-    <t>GARCÍA</t>
-  </si>
-  <si>
-    <t>Encarni</t>
-  </si>
-  <si>
-    <t>encarnacion.garcia@ieo.csic.es</t>
-  </si>
-  <si>
-    <t>ARA1-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GARRIGA PANISELLO</t>
-  </si>
-  <si>
-    <t>Mariona</t>
-  </si>
-  <si>
-    <t>mariona.garripa@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUR 5</t>
-  </si>
-  <si>
-    <t>KONRAD</t>
-  </si>
-  <si>
-    <t>Christoph</t>
-  </si>
-  <si>
-    <t>chriskon.official@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUT 9</t>
-  </si>
-  <si>
-    <t>LIGAS</t>
-  </si>
-  <si>
-    <t>Alessandro</t>
-  </si>
-  <si>
-    <t>ligas@cibm.it</t>
-  </si>
-  <si>
     <t>LOUIS</t>
   </si>
   <si>
@@ -195,111 +345,6 @@
     <t>louis.collin@developpement-durable.gouv.fr</t>
   </si>
   <si>
-    <t xml:space="preserve">DPS 1</t>
-  </si>
-  <si>
-    <t>MURENU</t>
-  </si>
-  <si>
-    <t>Matteo</t>
-  </si>
-  <si>
-    <t>mmurenu@unica.it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HKE 8-9-10-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HKE 8-9-10-11 &amp; MUT 10</t>
-  </si>
-  <si>
-    <t>MUSUMECI</t>
-  </si>
-  <si>
-    <t>Claudia</t>
-  </si>
-  <si>
-    <t>clamusu@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARA 8-9-10-11</t>
-  </si>
-  <si>
-    <t>ORIO</t>
-  </si>
-  <si>
-    <t>alessandro.orio@slu.se</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARS 8-9-10-11</t>
-  </si>
-  <si>
-    <t>PALERMINO</t>
-  </si>
-  <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>antonio.palermino@irbim.cnr.it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HKE 1-5-6-7  and HKE ad hoc?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HKE 1-5-6-7</t>
-  </si>
-  <si>
-    <t>PEREZ-RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>Alfonso</t>
-  </si>
-  <si>
-    <t>alfonso.perez@ieo.csic.es</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEP 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEP 11 &amp; MUR 5</t>
-  </si>
-  <si>
-    <t>SCANU</t>
-  </si>
-  <si>
-    <t>Martina</t>
-  </si>
-  <si>
-    <t>martina.scanu@irbim.cnr.it</t>
-  </si>
-  <si>
-    <t>spict</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEP 6</t>
-  </si>
-  <si>
-    <t>TIFOURA</t>
-  </si>
-  <si>
-    <t>Amina</t>
-  </si>
-  <si>
-    <t>amina.tifoura@ieo.csic.es</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARA 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZARAGOZA VILANOVA</t>
-  </si>
-  <si>
-    <t>NúRia</t>
-  </si>
-  <si>
-    <t>nuria.zaragoza@ieo.csic.es</t>
-  </si>
-  <si>
     <t>PIERUCCI</t>
   </si>
   <si>
@@ -307,37 +352,13 @@
   </si>
   <si>
     <t xml:space="preserve">Andrea.PIERUCCI@ec.europa.eu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DPS 5-6-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANTOPOULOU PALOUKA</t>
-  </si>
-  <si>
-    <t>DANAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Danai.MANTOPOULOU-PALOUKA@ec.europa.eu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUT 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RINCON HIDALGO</t>
-  </si>
-  <si>
-    <t>MARGHERITA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Margarita.RINCON-HIDALGO@ec.europa.eu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -347,6 +368,12 @@
       <u/>
       <sz val="11.000000"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -371,10 +398,24 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -894,12 +935,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.7109375"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" width="21.97265625"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" width="23.36328125"/>
-    <col customWidth="1" min="5" max="5" width="20.7109375"/>
-    <col customWidth="1" min="6" max="6" width="42.57421875"/>
-    <col customWidth="1" min="7" max="7" width="20.7109375"/>
+    <col customWidth="1" min="2" max="3" width="20.7109375"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="21.97265625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="23.36328125"/>
+    <col customWidth="1" min="6" max="6" width="20.7109375"/>
+    <col customWidth="1" min="7" max="7" width="42.57421875"/>
+    <col customWidth="1" min="8" max="8" width="20.7109375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25"/>
@@ -907,13 +948,13 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
@@ -922,479 +963,552 @@
       <c r="H2" t="s">
         <v>5</v>
       </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5"/>
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="G5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="B6"/>
-      <c r="C6"/>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6"/>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
-        <v>16</v>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" t="s">
-        <v>16</v>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9"/>
+        <v>34</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>36</v>
       </c>
+      <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="B10"/>
-      <c r="C10"/>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10"/>
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13"/>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3">
+        <v>11</v>
+      </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
+      <c r="B14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="B15"/>
-      <c r="C15"/>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15"/>
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16"/>
       <c r="E16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
+      <c r="B17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" t="s">
-        <v>16</v>
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
+      <c r="B20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
+      <c r="B22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="B23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" t="s">
-        <v>91</v>
-      </c>
+      <c r="B23"/>
+      <c r="C23" s="3"/>
+      <c r="D23"/>
       <c r="E23" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23"/>
     </row>
     <row r="24" ht="14.25">
       <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24"/>
+      <c r="C24" s="3"/>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25"/>
-      <c r="D25" t="s">
-        <v>98</v>
-      </c>
+      <c r="B25"/>
+      <c r="C25" s="3"/>
+      <c r="D25"/>
       <c r="E25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="B26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26"/>
-      <c r="D26" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="B26"/>
+      <c r="C26" s="3"/>
+      <c r="D26"/>
       <c r="E26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26"/>
     </row>
   </sheetData>
+  <sortState ref="B3:I26" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="C3:C26"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F3"/>
-    <hyperlink r:id="rId2" ref="F4"/>
-    <hyperlink r:id="rId3" ref="F5"/>
-    <hyperlink r:id="rId4" ref="F6"/>
-    <hyperlink r:id="rId5" ref="F7"/>
-    <hyperlink r:id="rId6" ref="F8"/>
-    <hyperlink r:id="rId7" ref="F9"/>
-    <hyperlink r:id="rId8" ref="F10"/>
-    <hyperlink r:id="rId9" ref="F11"/>
-    <hyperlink r:id="rId10" ref="F12"/>
-    <hyperlink r:id="rId11" ref="F13"/>
-    <hyperlink r:id="rId12" ref="F14"/>
-    <hyperlink r:id="rId13" ref="F15"/>
-    <hyperlink r:id="rId14" ref="F16"/>
-    <hyperlink r:id="rId15" ref="F17"/>
-    <hyperlink r:id="rId16" ref="F18"/>
-    <hyperlink r:id="rId17" ref="F19"/>
-    <hyperlink r:id="rId18" ref="F20"/>
-    <hyperlink r:id="rId19" ref="F21"/>
-    <hyperlink r:id="rId20" ref="F22"/>
-    <hyperlink r:id="rId21" ref="F23"/>
-    <hyperlink r:id="rId22" ref="F24"/>
-    <hyperlink r:id="rId23" ref="F25"/>
-    <hyperlink r:id="rId24" ref="F26"/>
+    <hyperlink r:id="rId1" ref="G3"/>
+    <hyperlink r:id="rId2" ref="G4"/>
+    <hyperlink r:id="rId3" ref="G5"/>
+    <hyperlink r:id="rId4" ref="G6"/>
+    <hyperlink r:id="rId5" ref="G7"/>
+    <hyperlink r:id="rId6" ref="G8"/>
+    <hyperlink r:id="rId7" ref="G9"/>
+    <hyperlink r:id="rId8" ref="G10"/>
+    <hyperlink r:id="rId9" ref="G11"/>
+    <hyperlink r:id="rId10" ref="G12"/>
+    <hyperlink r:id="rId11" ref="G13"/>
+    <hyperlink r:id="rId12" ref="G14"/>
+    <hyperlink r:id="rId13" ref="G15"/>
+    <hyperlink r:id="rId14" ref="G16"/>
+    <hyperlink r:id="rId15" ref="G17"/>
+    <hyperlink r:id="rId16" ref="G18"/>
+    <hyperlink r:id="rId17" ref="G19"/>
+    <hyperlink r:id="rId18" ref="G20"/>
+    <hyperlink r:id="rId19" ref="G21"/>
+    <hyperlink r:id="rId20" ref="G22"/>
+    <hyperlink r:id="rId21" ref="G23"/>
+    <hyperlink r:id="rId22" ref="G24"/>
+    <hyperlink r:id="rId23" ref="G25"/>
+    <hyperlink r:id="rId24" ref="G26"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>